<commit_message>
some try-and-error analysis on why H2 pipeline links are zero links_t.p0
</commit_message>
<xml_diff>
--- a/analysis files/configure_zero_links_t_p0.xlsx
+++ b/analysis files/configure_zero_links_t_p0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\work\pypsa_thesis\analysis files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFFAC3F-EC09-41CA-B73E-7933121CAC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF09645-7524-41DD-8258-9B219DAEE7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8BF64C96-22B0-4832-8BB8-F5804AF6748D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BF64C96-22B0-4832-8BB8-F5804AF6748D}"/>
   </bookViews>
   <sheets>
     <sheet name="2030 - TN-H2-G" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
   </si>
   <si>
     <t>i) even lower capital cost &amp; higher efficiency for H2 pipeline links, there are no links_t.p0 values for H2 pipelines
-ii) no requirement to utilize pipeline since operation of each electrolyzer to produce and meet H2 demand is sufficient already? Thus zero values for H2 pipeline links_t.p0?</t>
+ii) no requirement to utilize pipeline since operation of each electrolyzer, at each H2 bus/node, to produce and meet H2 demand is sufficient already? Thus zero values for H2 pipeline links_t.p0?</t>
   </si>
 </sst>
 </file>
@@ -295,64 +295,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CECF03-6EA7-4F36-B984-62B7AA50FCED}">
   <dimension ref="A2:P12"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,377 +694,377 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
+    <row r="5" spans="1:16" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>31</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>2030</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>3.24</v>
       </c>
-      <c r="F5" s="2">
-        <v>24</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="1">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.04</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="10">
         <v>0.66</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="10">
         <v>1</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="11">
         <v>32</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>2030</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>3.24</v>
       </c>
-      <c r="F6" s="2">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="1">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1">
         <v>0.04</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="10">
         <v>0.66</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="10">
         <v>1</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="N6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="17"/>
-      <c r="P6" s="20" t="s">
+      <c r="O6" s="9"/>
+      <c r="P6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="11">
         <v>33</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>2030</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>3.24</v>
       </c>
-      <c r="F7" s="2">
-        <v>24</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="1">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
         <v>0.04</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>0</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="10">
         <v>1</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="10">
         <v>1</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="17"/>
-      <c r="P7" s="20" t="s">
+      <c r="O7" s="9"/>
+      <c r="P7" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="11">
         <v>34</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>2030</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>3.24</v>
       </c>
-      <c r="F8" s="2">
-        <v>24</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="F8" s="1">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1">
         <v>0.04</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <v>0</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="10">
         <v>0.66</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="10">
         <v>1</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="O8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="A9" s="11">
         <v>35</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>2030</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>3.24</v>
       </c>
-      <c r="F9" s="2">
-        <v>24</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="1">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1">
         <v>0.04</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="3">
         <v>0</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="10">
         <v>1</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="10">
         <v>1</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="20" t="s">
+      <c r="O9" s="16"/>
+      <c r="P9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="11">
         <v>36</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>2030</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>3.24</v>
       </c>
-      <c r="F10" s="2">
-        <v>24</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="F10" s="1">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1">
         <v>0.04</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="3">
         <v>0</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="10">
         <v>0.66</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="10">
         <v>1</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="20" t="s">
+      <c r="O10" s="17"/>
+      <c r="P10" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="13"/>
       <c r="B12" t="s">
         <v>27</v>
       </c>
@@ -1095,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EFCED2-FC65-4454-A9CE-A6D33288E31F}">
   <dimension ref="A2:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1120,245 +1120,245 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
         <v>2040</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>28.3</v>
       </c>
-      <c r="F5" s="2">
-        <v>24</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="1">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.04</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="13"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1">
         <v>2040</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>28.3</v>
       </c>
-      <c r="F6" s="2">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="1">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1">
         <v>0.04</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="13"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1">
         <v>2040</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>28.3</v>
       </c>
-      <c r="F7" s="2">
-        <v>24</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="1">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
         <v>0.04</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="13"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1">
         <v>2040</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>28.3</v>
       </c>
-      <c r="F8" s="2">
-        <v>24</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="F8" s="1">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1">
         <v>0.04</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="7"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
         <v>2040</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>28.3</v>
       </c>
-      <c r="F9" s="2">
-        <v>24</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="1">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1">
         <v>0.04</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="7"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="5"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="13"/>
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -1413,245 +1413,245 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
         <v>2050</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>78.59</v>
       </c>
-      <c r="F5" s="2">
-        <v>24</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="1">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.04</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="13"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1">
         <v>2050</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>78.59</v>
       </c>
-      <c r="F6" s="2">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="1">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1">
         <v>0.04</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="13"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1">
         <v>2050</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>78.59</v>
       </c>
-      <c r="F7" s="2">
-        <v>24</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="1">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
         <v>0.04</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="13"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1">
         <v>2050</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>78.59</v>
       </c>
-      <c r="F8" s="2">
-        <v>24</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="F8" s="1">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1">
         <v>0.04</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="7"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
         <v>2050</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>78.59</v>
       </c>
-      <c r="F9" s="2">
-        <v>24</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="1">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1">
         <v>0.04</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="7"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="5"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="13"/>
       <c r="B11" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
testing to configure h2 pipe links zero with not all electrolyzers are installed
</commit_message>
<xml_diff>
--- a/analysis files/configure_zero_links_t_p0.xlsx
+++ b/analysis files/configure_zero_links_t_p0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\work\pypsa_thesis\analysis files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37414590-C1D5-42E9-9927-86E569606F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BACCE00-FA4B-4606-8347-06C5BDBFE3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{8BF64C96-22B0-4832-8BB8-F5804AF6748D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{8BF64C96-22B0-4832-8BB8-F5804AF6748D}"/>
   </bookViews>
   <sheets>
     <sheet name="2030 - TN-H2-G" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="48">
   <si>
     <t>Nyears</t>
   </si>
@@ -199,18 +199,15 @@
     <t>Length of (network.snapshots)</t>
   </si>
   <si>
-    <t>3 mins</t>
-  </si>
-  <si>
     <t>No. of H2 buses (with H2 Load)</t>
-  </si>
-  <si>
-    <t>12 mins</t>
   </si>
   <si>
     <t>infeasible model due to insufficient:
 1) total no. of electrolyzers?
 2) electrolyzer capacity to meet the H2 demand?</t>
+  </si>
+  <si>
+    <t>optimzation fail</t>
   </si>
 </sst>
 </file>
@@ -359,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,6 +401,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -419,47 +435,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,62 +801,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="18"/>
+      <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16" t="s">
+      <c r="M3" s="23"/>
+      <c r="N3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="16"/>
+      <c r="O3" s="23"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1085,7 +1083,7 @@
       <c r="O8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="22" t="s">
         <v>28</v>
       </c>
       <c r="Q8" s="12" t="s">
@@ -1138,7 +1136,7 @@
       <c r="O9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="23"/>
+      <c r="P9" s="22"/>
       <c r="Q9" s="12" t="s">
         <v>22</v>
       </c>
@@ -1189,7 +1187,7 @@
       <c r="O10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="23"/>
+      <c r="P10" s="22"/>
       <c r="Q10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1260,7 +1258,7 @@
       <c r="D12" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="17">
         <v>28.3</v>
       </c>
       <c r="F12" s="15" t="s">
@@ -1289,7 +1287,7 @@
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="21"/>
+      <c r="P12" s="16"/>
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1305,7 +1303,7 @@
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="17">
         <v>78.59</v>
       </c>
       <c r="F13" s="15" t="s">
@@ -1326,7 +1324,7 @@
       <c r="M13" s="10"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="21"/>
+      <c r="P13" s="16"/>
       <c r="Q13" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1337,6 +1335,7 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="P8:P10"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="J3:K3"/>
@@ -1350,7 +1349,6 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="P8:P10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1387,58 +1385,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="18"/>
+      <c r="N2" s="25"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16" t="s">
+      <c r="J3" s="23"/>
+      <c r="K3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="16"/>
+      <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1680,58 +1678,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="18"/>
+      <c r="N2" s="25"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16" t="s">
+      <c r="J3" s="23"/>
+      <c r="K3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="16"/>
+      <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1945,10 +1943,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862AEA04-81F6-492E-AE22-3C5C42470C12}">
-  <dimension ref="A2:R18"/>
+  <dimension ref="A2:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,74 +1972,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="19" t="s">
+      <c r="I3" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="16"/>
-      <c r="O3" s="24" t="s">
+      <c r="N3" s="23"/>
+      <c r="O3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="25" t="s">
+      <c r="P3" s="35"/>
+      <c r="Q3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="R3" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="14" t="s">
         <v>7</v>
       </c>
@@ -2060,12 +2058,12 @@
       <c r="P4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="28"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>37</v>
+      <c r="A5" s="18">
+        <v>40</v>
       </c>
       <c r="B5" s="15">
         <v>2030</v>
@@ -2092,7 +2090,7 @@
         <v>38</v>
       </c>
       <c r="J5" s="15">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K5" s="3">
         <v>3407.37</v>
@@ -2106,25 +2104,19 @@
       <c r="N5" s="10">
         <v>1</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
       <c r="R5" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>38</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>41</v>
       </c>
       <c r="B6" s="15">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>4</v>
@@ -2132,8 +2124,8 @@
       <c r="D6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="22">
-        <v>28.3</v>
+      <c r="E6" s="15">
+        <v>3.24</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>36</v>
@@ -2148,37 +2140,31 @@
         <v>38</v>
       </c>
       <c r="J6" s="15">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K6" s="3">
-        <v>2294.85</v>
+        <v>3407.37</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="M6" s="10">
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
       <c r="N6" s="10">
         <v>1</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="R6" s="32"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="33"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>39</v>
+      <c r="A7" s="18">
+        <v>42</v>
       </c>
       <c r="B7" s="15">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>4</v>
@@ -2186,8 +2172,8 @@
       <c r="D7" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="22">
-        <v>78.59</v>
+      <c r="E7" s="15">
+        <v>3.24</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>36</v>
@@ -2202,34 +2188,28 @@
         <v>38</v>
       </c>
       <c r="J7" s="15">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K7" s="3">
-        <v>2009.77</v>
+        <v>3407.37</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="M7" s="10">
-        <v>0.71</v>
+        <v>0.66</v>
       </c>
       <c r="N7" s="10">
         <v>1</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="R7" s="32"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="33"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
-        <v>40</v>
+      <c r="A8" s="18">
+        <v>43</v>
       </c>
       <c r="B8" s="15">
         <v>2030</v>
@@ -2256,7 +2236,7 @@
         <v>38</v>
       </c>
       <c r="J8" s="15">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K8" s="3">
         <v>3407.37</v>
@@ -2270,16 +2250,14 @@
       <c r="N8" s="10">
         <v>1</v>
       </c>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="28" t="s">
-        <v>48</v>
-      </c>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="34"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>41</v>
+      <c r="A9" s="11">
+        <v>44</v>
       </c>
       <c r="B9" s="15">
         <v>2030</v>
@@ -2306,7 +2284,7 @@
         <v>38</v>
       </c>
       <c r="J9" s="15">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K9" s="3">
         <v>3407.37</v>
@@ -2320,17 +2298,19 @@
       <c r="N9" s="10">
         <v>1</v>
       </c>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="29"/>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="30" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>45</v>
+      </c>
       <c r="B10" s="15">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>4</v>
@@ -2338,8 +2318,8 @@
       <c r="D10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="15">
-        <v>3.24</v>
+      <c r="E10" s="17">
+        <v>28.3</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>36</v>
@@ -2354,31 +2334,31 @@
         <v>38</v>
       </c>
       <c r="J10" s="15">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K10" s="3">
-        <v>3407.37</v>
+        <v>2294.85</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="M10" s="10">
-        <v>0.66</v>
+        <v>0.68</v>
       </c>
       <c r="N10" s="10">
         <v>1</v>
       </c>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="29"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="30"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31">
-        <v>43</v>
+      <c r="A11" s="11">
+        <v>46</v>
       </c>
       <c r="B11" s="15">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>4</v>
@@ -2386,8 +2366,8 @@
       <c r="D11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="15">
-        <v>3.24</v>
+      <c r="E11" s="17">
+        <v>78.59</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>36</v>
@@ -2402,28 +2382,28 @@
         <v>38</v>
       </c>
       <c r="J11" s="15">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K11" s="3">
-        <v>3407.37</v>
+        <v>2009.77</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="M11" s="10">
-        <v>0.66</v>
+        <v>0.71</v>
       </c>
       <c r="N11" s="10">
         <v>1</v>
       </c>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="15"/>
       <c r="R11" s="30"/>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B12" s="15">
         <v>2030</v>
@@ -2455,8 +2435,8 @@
       <c r="K12" s="3">
         <v>3407.37</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>32</v>
+      <c r="L12" s="3">
+        <v>0.1</v>
       </c>
       <c r="M12" s="10">
         <v>0.66</v>
@@ -2467,16 +2447,14 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="15"/>
-      <c r="R12" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="20"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13" s="15">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>4</v>
@@ -2484,8 +2462,8 @@
       <c r="D13" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="22">
-        <v>28.3</v>
+      <c r="E13" s="15">
+        <v>3.24</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>36</v>
@@ -2500,16 +2478,16 @@
         <v>38</v>
       </c>
       <c r="J13" s="15">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="K13" s="3">
-        <v>2294.85</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>37</v>
+        <v>3407.37</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.1</v>
       </c>
       <c r="M13" s="10">
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
       <c r="N13" s="10">
         <v>1</v>
@@ -2517,166 +2495,27 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="15"/>
-      <c r="R13" s="32"/>
-    </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
-        <v>46</v>
-      </c>
-      <c r="B14" s="15">
-        <v>2050</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="22">
-        <v>78.59</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="15">
-        <v>365</v>
-      </c>
-      <c r="H14" s="15">
-        <v>158</v>
-      </c>
-      <c r="I14" s="15">
-        <v>38</v>
-      </c>
-      <c r="J14" s="15">
-        <v>19</v>
-      </c>
-      <c r="K14" s="3">
-        <v>2009.77</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" s="10">
-        <v>0.71</v>
-      </c>
-      <c r="N14" s="10">
-        <v>1</v>
-      </c>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="32"/>
-    </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="R13" s="20"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="15">
-        <v>2030</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="15">
-        <v>3.24</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="15">
-        <v>365</v>
-      </c>
-      <c r="H15" s="15">
-        <v>158</v>
-      </c>
-      <c r="I15" s="15">
-        <v>38</v>
-      </c>
-      <c r="J15" s="15">
-        <v>19</v>
-      </c>
-      <c r="K15" s="3">
-        <v>3407.37</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M15" s="10">
-        <v>0.66</v>
-      </c>
-      <c r="N15" s="10">
-        <v>1</v>
-      </c>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="34"/>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>48</v>
-      </c>
-      <c r="B16" s="15">
-        <v>2030</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="15">
-        <v>3.24</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="15">
-        <v>365</v>
-      </c>
-      <c r="H16" s="15">
-        <v>158</v>
-      </c>
-      <c r="I16" s="15">
-        <v>38</v>
-      </c>
-      <c r="J16" s="15">
-        <v>38</v>
-      </c>
-      <c r="K16" s="3">
-        <v>3407.37</v>
-      </c>
-      <c r="L16" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M16" s="10">
-        <v>0.66</v>
-      </c>
-      <c r="N16" s="10">
-        <v>1</v>
-      </c>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="34"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="R12:R14"/>
+  <mergeCells count="18">
+    <mergeCell ref="R9:R11"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="R5:R7"/>
-    <mergeCell ref="R8:R11"/>
+    <mergeCell ref="R5:R8"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>

</xml_diff>

<commit_message>
configure zero values for H2 pipeline links, test with partial no. of electrolyzers
</commit_message>
<xml_diff>
--- a/analysis files/configure_zero_links_t_p0.xlsx
+++ b/analysis files/configure_zero_links_t_p0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\work\pypsa_thesis\analysis files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BACCE00-FA4B-4606-8347-06C5BDBFE3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26AA223-5E48-4E38-89E1-9706FC8A569B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{8BF64C96-22B0-4832-8BB8-F5804AF6748D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="59">
   <si>
     <t>Nyears</t>
   </si>
@@ -184,22 +184,10 @@
     <t>optimization solved in</t>
   </si>
   <si>
-    <t>No. of Electrolyzers</t>
-  </si>
-  <si>
     <t>range 4 - 39</t>
   </si>
   <si>
     <t>there are transportation of H2 between H2 pipelines to meet H2 demand at all H2 buses</t>
-  </si>
-  <si>
-    <t>No. of AC buses</t>
-  </si>
-  <si>
-    <t>Length of (network.snapshots)</t>
-  </si>
-  <si>
-    <t>No. of H2 buses (with H2 Load)</t>
   </si>
   <si>
     <t>infeasible model due to insufficient:
@@ -208,6 +196,51 @@
   </si>
   <si>
     <t>optimzation fail</t>
+  </si>
+  <si>
+    <t>5 mins</t>
+  </si>
+  <si>
+    <t>7 mins</t>
+  </si>
+  <si>
+    <t>14 mins</t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>remarks / assumptions</t>
+  </si>
+  <si>
+    <t>after successful optimization</t>
+  </si>
+  <si>
+    <t>electrolysis</t>
+  </si>
+  <si>
+    <t>capital cost [EUR/MW]</t>
+  </si>
+  <si>
+    <t>no. of electrolyzers</t>
+  </si>
+  <si>
+    <t>no. of H2 Buses (with H2 Load)</t>
+  </si>
+  <si>
+    <t>no. of AC Buses</t>
+  </si>
+  <si>
+    <t>length of (network.snapshots)</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>electrolyzers at each H2 bus is sufficient to meet the H2 demand. no need H2 transportation between the buses via H2 pipelines</t>
   </si>
 </sst>
 </file>
@@ -413,8 +446,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -440,9 +476,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -801,62 +834,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="25"/>
+      <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="23"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1083,7 +1116,7 @@
       <c r="O8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="P8" s="23" t="s">
         <v>28</v>
       </c>
       <c r="Q8" s="12" t="s">
@@ -1136,7 +1169,7 @@
       <c r="O9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="22"/>
+      <c r="P9" s="23"/>
       <c r="Q9" s="12" t="s">
         <v>22</v>
       </c>
@@ -1187,7 +1220,7 @@
       <c r="O10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="22"/>
+      <c r="P10" s="23"/>
       <c r="Q10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1385,58 +1418,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="25"/>
+      <c r="N2" s="26"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="23"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1678,58 +1711,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="25"/>
+      <c r="N2" s="26"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="23"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1946,7 +1979,7 @@
   <dimension ref="A2:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,94 +2005,94 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
+      <c r="O2" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>44</v>
+      <c r="F3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>56</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="23"/>
+      <c r="N3" s="24"/>
       <c r="O3" s="35" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="35"/>
-      <c r="Q3" s="29" t="s">
+      <c r="Q3" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="28" t="s">
-        <v>14</v>
+      <c r="R3" s="29" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="14" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="14" t="s">
+      <c r="M4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="20" t="s">
         <v>8</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="28"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="29"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
@@ -2108,7 +2141,7 @@
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
       <c r="R5" s="32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,11 +2331,17 @@
       <c r="N9" s="10">
         <v>1</v>
       </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="30" t="s">
-        <v>42</v>
+      <c r="O9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="R9" s="32" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2348,10 +2387,16 @@
       <c r="N10" s="10">
         <v>1</v>
       </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="30"/>
+      <c r="O10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="R10" s="33"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
@@ -2388,7 +2433,7 @@
         <v>2009.77</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M11" s="10">
         <v>0.71</v>
@@ -2396,10 +2441,16 @@
       <c r="N11" s="10">
         <v>1</v>
       </c>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="30"/>
+      <c r="O11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="R11" s="33"/>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -2444,12 +2495,18 @@
       <c r="N12" s="10">
         <v>1</v>
       </c>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="20"/>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="R12" s="34"/>
+    </row>
+    <row r="13" spans="1:18" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>48</v>
       </c>
@@ -2492,10 +2549,18 @@
       <c r="N13" s="10">
         <v>1</v>
       </c>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="20"/>
+      <c r="O13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
@@ -2504,14 +2569,13 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="R9:R11"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="G3:G4"/>
@@ -2519,6 +2583,7 @@
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
+    <mergeCell ref="R9:R12"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="A3:A4"/>

</xml_diff>